<commit_message>
Add logs to create fake service and create fake event #419 Add category to create new services #423 added missing features and users have more than one interest
</commit_message>
<xml_diff>
--- a/social/management/commands/interest_example.xlsx
+++ b/social/management/commands/interest_example.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FDFDC16-98DB-4F5F-8D1C-0F53F67E1ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AC58FF9-FB65-4569-BB3F-F5D512C3704E}" xr6:coauthVersionLast="48" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sayfa1!$B$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -38,79 +41,280 @@
     <t>wiki_description</t>
   </si>
   <si>
+    <t>airplanes</t>
+  </si>
+  <si>
+    <t>powered fixed-wing aircraft</t>
+  </si>
+  <si>
+    <t>anime</t>
+  </si>
+  <si>
+    <t>Japanese animation</t>
+  </si>
+  <si>
+    <t>astronomy</t>
+  </si>
+  <si>
+    <t>natural science that deals with the study of celestial objects</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>team sport played on a court with baskets on either end</t>
+  </si>
+  <si>
+    <t>bicycle</t>
+  </si>
+  <si>
+    <t>pedal-driven two-wheel vehicle</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>road vehicle powered by a motor to carry driver and small number of passengers</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>domesticated feline</t>
+  </si>
+  <si>
+    <t>cha cha</t>
+  </si>
+  <si>
+    <t>dance of Cuban origin</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>general-purpose device for performing arithmetic or logical operations</t>
+  </si>
+  <si>
+    <t>cooking</t>
+  </si>
+  <si>
+    <t>preparing food for consumption by the application of heat</t>
+  </si>
+  <si>
+    <t>diabolo</t>
+  </si>
+  <si>
+    <t>Juggling prop</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>domestic animal</t>
+  </si>
+  <si>
+    <t>everest</t>
+  </si>
+  <si>
+    <t>Earth's highest mountain above sea level, located in the Mahalangur Himal sub-range of the Himalayas</t>
+  </si>
+  <si>
+    <t>fantasy role playing</t>
+  </si>
+  <si>
+    <t>game in which players assume the roles of characters in a fictional setting. Use Tabletop role-playing game (Q1643932) for the leasure activity.</t>
+  </si>
+  <si>
+    <t>fishing</t>
+  </si>
+  <si>
+    <t>activity of trying to catch fish</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>sport that is practiced between two teams of eleven players</t>
+  </si>
+  <si>
+    <t>fps</t>
+  </si>
+  <si>
+    <t>video game genre centered around gun and other weapon-based combat in a first-person perspective</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>electronic game that involves interaction with a user interface to generate visual feedback on a video device such as a TV screen or computer monitor</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>fretted string instrument</t>
+  </si>
+  <si>
+    <t>harry potter</t>
+  </si>
+  <si>
+    <t>series of fantasy novels by J.K. Rowling</t>
+  </si>
+  <si>
+    <t>horon</t>
+  </si>
+  <si>
+    <t>type of dance</t>
+  </si>
+  <si>
+    <t>içli köfte</t>
+  </si>
+  <si>
+    <t>dumplings made of bulgur with ground meat and onions</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>musical genre and theory</t>
+  </si>
+  <si>
+    <t>juggling</t>
+  </si>
+  <si>
+    <t>circus skill</t>
+  </si>
+  <si>
+    <t>prop used in juggling</t>
+  </si>
+  <si>
+    <t>kebab</t>
+  </si>
+  <si>
+    <t>class of roasted meat dishes in Turkey and Middle East</t>
+  </si>
+  <si>
+    <t>lord of the rings</t>
+  </si>
+  <si>
+    <t>1954–1955 fantasy novel by J. R. R. Tolkien</t>
+  </si>
+  <si>
+    <t>manga</t>
+  </si>
+  <si>
+    <t>comics or graphic novels created in Japan</t>
+  </si>
+  <si>
+    <t>minerals</t>
+  </si>
+  <si>
+    <t>naturally occurring usually inorganic substance that has a (more or less) definite chemical composition and a crystal structure</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>art form, and cultural activity, whose medium is sound</t>
+  </si>
+  <si>
+    <t>olympics</t>
+  </si>
+  <si>
+    <t>major international sport event</t>
+  </si>
+  <si>
+    <t>painting</t>
+  </si>
+  <si>
+    <t>practice of applying paint, pigment, color or other medium to a surface</t>
+  </si>
+  <si>
+    <t>pigeon</t>
+  </si>
+  <si>
+    <t>family of birds</t>
+  </si>
+  <si>
+    <t>pilates</t>
+  </si>
+  <si>
+    <t>physical fitness system</t>
+  </si>
+  <si>
+    <t>poetry</t>
+  </si>
+  <si>
+    <t>literary style characterized by a strong expressiveness of words</t>
+  </si>
+  <si>
+    <t>poi</t>
+  </si>
+  <si>
+    <t>balls swung rhythmically on strings</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>the process of designing and building an executable computer program to accomplish a specific computing result or to perform a specific task</t>
+  </si>
+  <si>
+    <t>recorder</t>
+  </si>
+  <si>
+    <t>woodwind musical instrument</t>
+  </si>
+  <si>
+    <t>reiki</t>
+  </si>
+  <si>
+    <t>Pseudoscientific Japanese alternative medicine similar to laying on of hands</t>
+  </si>
+  <si>
+    <t>salsa</t>
+  </si>
+  <si>
+    <t>dance form</t>
+  </si>
+  <si>
+    <t>scuba</t>
+  </si>
+  <si>
+    <t>Swimming underwater breathing gas carried by the diver</t>
+  </si>
+  <si>
     <t>snooker</t>
   </si>
   <si>
     <t>cue sport</t>
   </si>
   <si>
-    <t>poi</t>
-  </si>
-  <si>
-    <t>balls swung rhythmically on strings</t>
-  </si>
-  <si>
-    <t>airplanes</t>
-  </si>
-  <si>
-    <t>powered fixed-wing aircraft</t>
-  </si>
-  <si>
     <t>sports</t>
   </si>
   <si>
     <t>forms of competitive physical activity or games which, through casual or organized participation, maintain or improve physical ability and skills while providing enjoyment to participants, and in some cases, entertainment for spectators</t>
   </si>
   <si>
-    <t>computer</t>
-  </si>
-  <si>
-    <t>general-purpose device for performing arithmetic or logical operations</t>
-  </si>
-  <si>
-    <t>juggling</t>
-  </si>
-  <si>
-    <t>circus skill</t>
-  </si>
-  <si>
-    <t>prop used in juggling</t>
-  </si>
-  <si>
-    <t>game</t>
-  </si>
-  <si>
-    <t>electronic game that involves interaction with a user interface to generate visual feedback on a video device such as a TV screen or computer monitor</t>
-  </si>
-  <si>
-    <t>poetry</t>
-  </si>
-  <si>
-    <t>literary style characterized by a strong expressiveness of words</t>
-  </si>
-  <si>
-    <t>programming</t>
-  </si>
-  <si>
-    <t>the process of designing and building an executable computer program to accomplish a specific computing result or to perform a specific task</t>
-  </si>
-  <si>
-    <t>music</t>
-  </si>
-  <si>
-    <t>art form, and cultural activity, whose medium is sound</t>
-  </si>
-  <si>
-    <t>jazz</t>
-  </si>
-  <si>
-    <t>musical genre and theory</t>
-  </si>
-  <si>
-    <t>guitar</t>
-  </si>
-  <si>
-    <t>fretted string instrument</t>
+    <t>straw</t>
+  </si>
+  <si>
+    <t>agricultural by-product</t>
+  </si>
+  <si>
+    <t>straw hat</t>
+  </si>
+  <si>
+    <t>fictional character from One Piece</t>
+  </si>
+  <si>
+    <t>fictional pirate group from One Piece</t>
+  </si>
+  <si>
+    <t>ukulele</t>
+  </si>
+  <si>
+    <t>member of the guitar family</t>
   </si>
   <si>
     <t>violin</t>
@@ -119,97 +323,10 @@
     <t>bowed string instrument, usually with four strings tuned in perfect fifths</t>
   </si>
   <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>domestic animal</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>domesticated feline</t>
-  </si>
-  <si>
-    <t>cooking</t>
-  </si>
-  <si>
-    <t>preparing food for consumption by the application of heat</t>
-  </si>
-  <si>
-    <t>kebab</t>
-  </si>
-  <si>
-    <t>class of roasted meat dishes in Turkey and Middle East</t>
-  </si>
-  <si>
-    <t>football</t>
-  </si>
-  <si>
-    <t>sport that is practiced between two teams of eleven players</t>
-  </si>
-  <si>
-    <t>basketball</t>
-  </si>
-  <si>
-    <t>team sport played on a court with baskets on either end</t>
-  </si>
-  <si>
-    <t>scuba</t>
-  </si>
-  <si>
-    <t>Swimming underwater breathing gas carried by the diver</t>
-  </si>
-  <si>
-    <t>fantasy role playing</t>
-  </si>
-  <si>
-    <t>game in which players assume the roles of characters in a fictional setting. Use Tabletop role-playing game (Q1643932) for the leasure activity.</t>
-  </si>
-  <si>
-    <t>ukulele</t>
-  </si>
-  <si>
-    <t>member of the guitar family</t>
-  </si>
-  <si>
-    <t>fishing</t>
-  </si>
-  <si>
-    <t>activity of trying to catch fish</t>
-  </si>
-  <si>
-    <t>diabolo</t>
-  </si>
-  <si>
-    <t>Juggling prop</t>
-  </si>
-  <si>
-    <t>içli köfte</t>
-  </si>
-  <si>
-    <t>dumplings made of bulgur with ground meat and onions</t>
-  </si>
-  <si>
-    <t>straw</t>
-  </si>
-  <si>
-    <t>agricultural by-product</t>
-  </si>
-  <si>
-    <t>straw hat</t>
-  </si>
-  <si>
-    <t>fictional character from One Piece</t>
-  </si>
-  <si>
-    <t>fictional pirate group from One Piece</t>
-  </si>
-  <si>
-    <t>everest</t>
-  </si>
-  <si>
-    <t>Earth's highest mountain above sea level, located in the Mahalangur Himal sub-range of the Himalayas</t>
+    <t>yoga</t>
+  </si>
+  <si>
+    <t>group of physical, mental and spiritual practices originating from ancient India</t>
   </si>
 </sst>
 </file>
@@ -561,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -651,10 +768,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -662,10 +779,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -673,10 +790,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -684,10 +801,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -695,10 +812,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -706,10 +823,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -717,10 +834,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -728,10 +845,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -739,10 +856,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -750,10 +867,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -761,10 +878,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -772,10 +889,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -783,10 +900,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -794,10 +911,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -805,10 +922,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -816,10 +933,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -827,10 +944,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -838,10 +955,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -849,7 +966,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>51</v>
@@ -860,10 +977,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -871,10 +988,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -882,10 +999,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -893,10 +1010,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -904,10 +1021,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -915,13 +1032,227 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C51">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>